<commit_message>
Finished the second part where implement the funciotns or methods for the 7 activities
</commit_message>
<xml_diff>
--- a/nba2.xlsx
+++ b/nba2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\Hitch\Tech_Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bucar\Documents\Tech_Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68D1AAE-E470-4441-AF87-B2DEFF764CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A24074-3FC4-45C2-8E82-A8CEC4753B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2595" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nba" sheetId="1" r:id="rId1"/>
@@ -1762,12 +1762,14 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -1825,7 +1827,7 @@
         <v>2250000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>241</v>
       </c>
@@ -1854,7 +1856,7 @@
         <v>4171680</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -1883,7 +1885,7 @@
         <v>525093</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -1912,7 +1914,7 @@
         <v>1938840</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>219</v>
       </c>
@@ -1941,7 +1943,7 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>224</v>
       </c>
@@ -1967,7 +1969,7 @@
         <v>13500000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>251</v>
       </c>
@@ -1996,7 +1998,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -2025,7 +2027,7 @@
         <v>83397</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>292</v>
       </c>
@@ -2054,7 +2056,7 @@
         <v>9463484</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -2083,7 +2085,7 @@
         <v>3807120</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>199</v>
       </c>
@@ -2135,7 +2137,7 @@
         <v>4389607</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>279</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v>8042895</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>280</v>
       </c>
@@ -2193,7 +2195,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>208</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>1320000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>232</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2274,7 +2276,7 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -2300,7 +2302,7 @@
         <v>289755</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -2329,7 +2331,7 @@
         <v>3272091</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -2358,7 +2360,7 @@
         <v>11710456</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -2387,7 +2389,7 @@
         <v>250750</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>275</v>
       </c>
@@ -2416,7 +2418,7 @@
         <v>1210800</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -2445,7 +2447,7 @@
         <v>13800000</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>186</v>
       </c>
@@ -2474,7 +2476,7 @@
         <v>200600</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>246</v>
       </c>
@@ -2503,7 +2505,7 @@
         <v>2380593</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>270</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>5758680</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>106</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>203</v>
       </c>
@@ -2590,7 +2592,7 @@
         <v>7070730</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>273</v>
       </c>
@@ -2619,7 +2621,7 @@
         <v>3344000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>156</v>
       </c>
@@ -2648,7 +2650,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>113</v>
       </c>
@@ -2677,7 +2679,7 @@
         <v>1160160</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -2735,7 +2737,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>3110796</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2793,7 +2795,7 @@
         <v>7730337</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>264</v>
       </c>
@@ -2816,7 +2818,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -2845,7 +2847,7 @@
         <v>3156600</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -2871,7 +2873,7 @@
         <v>2814000</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>98</v>
       </c>
@@ -2900,7 +2902,7 @@
         <v>18907726</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>214</v>
       </c>
@@ -2926,7 +2928,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>139</v>
       </c>
@@ -2955,7 +2957,7 @@
         <v>1391160</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>3425510</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>212</v>
       </c>
@@ -3007,7 +3009,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>253</v>
       </c>
@@ -3036,7 +3038,7 @@
         <v>5694674</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>198</v>
       </c>
@@ -3065,7 +3067,7 @@
         <v>5464000</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>525093</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -3123,7 +3125,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -3149,7 +3151,7 @@
         <v>8344497</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>114</v>
       </c>
@@ -3178,7 +3180,7 @@
         <v>13500000</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -3207,7 +3209,7 @@
         <v>1270964</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>289</v>
       </c>
@@ -3236,7 +3238,7 @@
         <v>2854940</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>234</v>
       </c>
@@ -3262,7 +3264,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v>19689000</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>1524000</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>194</v>
       </c>
@@ -3346,7 +3348,7 @@
         <v>700902</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>204</v>
       </c>
@@ -3375,7 +3377,7 @@
         <v>169883</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>287</v>
       </c>
@@ -3404,7 +3406,7 @@
         <v>2525160</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>162</v>
       </c>
@@ -3430,7 +3432,7 @@
         <v>4394225</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>250</v>
       </c>
@@ -3459,7 +3461,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>103</v>
       </c>
@@ -3488,7 +3490,7 @@
         <v>1159680</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>130</v>
       </c>
@@ -3517,7 +3519,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>274</v>
       </c>
@@ -3546,7 +3548,7 @@
         <v>2021520</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -3575,7 +3577,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -3604,7 +3606,7 @@
         <v>22875000</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>122</v>
       </c>
@@ -3633,7 +3635,7 @@
         <v>1449187</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>178</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>15361500</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>144</v>
       </c>
@@ -3691,7 +3693,7 @@
         <v>8193029</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>180</v>
       </c>
@@ -3720,7 +3722,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -3749,7 +3751,7 @@
         <v>206192</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>192</v>
       </c>
@@ -3778,7 +3780,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>228</v>
       </c>
@@ -3807,7 +3809,7 @@
         <v>22192730</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>297</v>
       </c>
@@ -3836,7 +3838,7 @@
         <v>981348</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>283</v>
       </c>
@@ -3865,7 +3867,7 @@
         <v>5016000</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>37</v>
       </c>
@@ -3894,7 +3896,7 @@
         <v>1140240</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>101</v>
       </c>
@@ -3923,7 +3925,7 @@
         <v>21468695</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>65</v>
       </c>
@@ -3952,7 +3954,7 @@
         <v>525093</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>49</v>
       </c>
@@ -3981,7 +3983,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>277</v>
       </c>
@@ -4010,7 +4012,7 @@
         <v>525093</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>185</v>
       </c>
@@ -4036,7 +4038,7 @@
         <v>1242720</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>227</v>
       </c>
@@ -4065,7 +4067,7 @@
         <v>4204200</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -4094,7 +4096,7 @@
         <v>1100602</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>184</v>
       </c>
@@ -4123,7 +4125,7 @@
         <v>8229375</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>74</v>
       </c>
@@ -4152,7 +4154,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>226</v>
       </c>
@@ -4181,7 +4183,7 @@
         <v>5675000</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>135</v>
       </c>
@@ -4207,7 +4209,7 @@
         <v>525093</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>258</v>
       </c>
@@ -4236,7 +4238,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -4262,7 +4264,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>285</v>
       </c>
@@ -4291,7 +4293,7 @@
         <v>4236287</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>167</v>
       </c>
@@ -4317,7 +4319,7 @@
         <v>855000</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>268</v>
       </c>
@@ -4343,7 +4345,7 @@
         <v>1149500</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -4372,7 +4374,7 @@
         <v>5103120</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>259</v>
       </c>
@@ -4398,7 +4400,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>213</v>
       </c>
@@ -4427,7 +4429,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -4456,7 +4458,7 @@
         <v>2850000</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>293</v>
       </c>
@@ -4482,7 +4484,7 @@
         <v>3777720</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>256</v>
       </c>
@@ -4511,7 +4513,7 @@
         <v>2814000</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>124</v>
       </c>
@@ -4540,7 +4542,7 @@
         <v>5013559</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>155</v>
       </c>
@@ -4569,7 +4571,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>176</v>
       </c>
@@ -4598,7 +4600,7 @@
         <v>2085671</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>216</v>
       </c>
@@ -4627,7 +4629,7 @@
         <v>1499187</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -4656,7 +4658,7 @@
         <v>19689000</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>76</v>
       </c>
@@ -4685,7 +4687,7 @@
         <v>1509360</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>71</v>
       </c>
@@ -4714,7 +4716,7 @@
         <v>10050000</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>125</v>
       </c>
@@ -4743,7 +4745,7 @@
         <v>15851950</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>69</v>
       </c>
@@ -4772,7 +4774,7 @@
         <v>13600000</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>220</v>
       </c>
@@ -4798,7 +4800,7 @@
         <v>1763400</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>181</v>
       </c>
@@ -4827,7 +4829,7 @@
         <v>5378974</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>294</v>
       </c>
@@ -4856,7 +4858,7 @@
         <v>12000000</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>141</v>
       </c>
@@ -4885,7 +4887,7 @@
         <v>20093064</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>53</v>
       </c>
@@ -4914,7 +4916,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -4943,7 +4945,7 @@
         <v>2127840</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>175</v>
       </c>
@@ -4972,7 +4974,7 @@
         <v>4053446</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>244</v>
       </c>
@@ -5001,7 +5003,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -5030,7 +5032,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>276</v>
       </c>
@@ -5059,7 +5061,7 @@
         <v>5138430</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>177</v>
       </c>
@@ -5085,7 +5087,7 @@
         <v>8333334</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>42</v>
       </c>
@@ -5114,7 +5116,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>190</v>
       </c>
@@ -5140,7 +5142,7 @@
         <v>2288205</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>237</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -5192,7 +5194,7 @@
         <v>2380440</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>85</v>
       </c>
@@ -5221,7 +5223,7 @@
         <v>14260870</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>254</v>
       </c>
@@ -5250,7 +5252,7 @@
         <v>3300000</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>126</v>
       </c>
@@ -5279,7 +5281,7 @@
         <v>525093</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>189</v>
       </c>
@@ -5305,7 +5307,7 @@
         <v>22359364</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>179</v>
       </c>
@@ -5334,7 +5336,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>233</v>
       </c>
@@ -5363,7 +5365,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>281</v>
       </c>
@@ -5392,7 +5394,7 @@
         <v>6980802</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>248</v>
       </c>
@@ -5421,7 +5423,7 @@
         <v>2505720</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>54</v>
       </c>
@@ -5447,7 +5449,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>261</v>
       </c>
@@ -5473,7 +5475,7 @@
         <v>3102240</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>272</v>
       </c>
@@ -5502,7 +5504,7 @@
         <v>16407500</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>109</v>
       </c>
@@ -5531,7 +5533,7 @@
         <v>13500000</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>209</v>
       </c>
@@ -5560,7 +5562,7 @@
         <v>15514031</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>128</v>
       </c>
@@ -5589,7 +5591,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>242</v>
       </c>
@@ -5615,7 +5617,7 @@
         <v>7900000</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>138</v>
       </c>
@@ -5644,7 +5646,7 @@
         <v>1015421</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>240</v>
       </c>
@@ -5670,7 +5672,7 @@
         <v>2288205</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -5699,7 +5701,7 @@
         <v>3425510</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>83</v>
       </c>
@@ -5728,7 +5730,7 @@
         <v>2008748</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>225</v>
       </c>
@@ -5757,7 +5759,7 @@
         <v>2612520</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>255</v>
       </c>
@@ -5786,7 +5788,7 @@
         <v>1100602</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>260</v>
       </c>
@@ -5815,7 +5817,7 @@
         <v>1584480</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>159</v>
       </c>
@@ -5844,7 +5846,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>231</v>
       </c>
@@ -5870,7 +5872,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>282</v>
       </c>
@@ -5899,7 +5901,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>164</v>
       </c>
@@ -5925,7 +5927,7 @@
         <v>1953960</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>163</v>
       </c>
@@ -5954,7 +5956,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>230</v>
       </c>
@@ -5980,7 +5982,7 @@
         <v>14783000</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>295</v>
       </c>
@@ -6009,7 +6011,7 @@
         <v>15409570</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>266</v>
       </c>
@@ -6038,7 +6040,7 @@
         <v>1474440</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>168</v>
       </c>
@@ -6067,7 +6069,7 @@
         <v>16407500</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>269</v>
       </c>
@@ -6093,7 +6095,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>170</v>
       </c>
@@ -6122,7 +6124,7 @@
         <v>6600000</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>79</v>
       </c>
@@ -6151,7 +6153,7 @@
         <v>3873398</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>235</v>
       </c>
@@ -6180,7 +6182,7 @@
         <v>981348</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>40</v>
       </c>
@@ -6209,7 +6211,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>64</v>
       </c>
@@ -6238,7 +6240,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>81</v>
       </c>
@@ -6267,7 +6269,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -6293,7 +6295,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>148</v>
       </c>
@@ -6322,7 +6324,7 @@
         <v>8988765</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>56</v>
       </c>
@@ -6351,7 +6353,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>24</v>
       </c>
@@ -6380,7 +6382,7 @@
         <v>6912869</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>61</v>
       </c>
@@ -6409,7 +6411,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -6438,7 +6440,7 @@
         <v>4290000</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>149</v>
       </c>
@@ -6464,7 +6466,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>169</v>
       </c>
@@ -6493,7 +6495,7 @@
         <v>5152440</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>13</v>
       </c>
@@ -6522,7 +6524,7 @@
         <v>6796117</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>60</v>
       </c>
@@ -6551,7 +6553,7 @@
         <v>4582680</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>263</v>
       </c>
@@ -6580,7 +6582,7 @@
         <v>258489</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>96</v>
       </c>
@@ -6609,7 +6611,7 @@
         <v>5675000</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>262</v>
       </c>
@@ -6638,7 +6640,7 @@
         <v>4345000</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>121</v>
       </c>
@@ -6667,7 +6669,7 @@
         <v>1015421</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>206</v>
       </c>
@@ -6696,7 +6698,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>188</v>
       </c>
@@ -6725,7 +6727,7 @@
         <v>15756438</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>73</v>
       </c>
@@ -6754,7 +6756,7 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>146</v>
       </c>
@@ -6783,7 +6785,7 @@
         <v>947276</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>88</v>
       </c>
@@ -6812,7 +6814,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>27</v>
       </c>
@@ -6841,7 +6843,7 @@
         <v>1749840</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>196</v>
       </c>
@@ -6870,7 +6872,7 @@
         <v>845059</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>166</v>
       </c>

</xml_diff>